<commit_message>
Complete Lab 9 report
</commit_message>
<xml_diff>
--- a/Lab Reports/LabReport7/PHY121 - Lab 7 - Data.xlsx
+++ b/Lab Reports/LabReport7/PHY121 - Lab 7 - Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abereni4u/Dropbox/Github/PHY121/Lab Reports/LabReport7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7F240A-2E2A-CD41-AE9C-6FBEE28A2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA49E22-9402-F84F-BF10-A88894DE429F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -357,9 +357,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -382,13 +381,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,7 +1226,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1265,7 +1263,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -1517,7 +1515,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1554,7 +1552,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1629,7 +1627,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1658,7 +1656,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2983,11 +2981,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:D50"/>
+    <sheetView topLeftCell="A26" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
@@ -2995,12 +2993,12 @@
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3011,558 +3009,558 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="1:7">
+      <c r="C9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
         <v>1000</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <f>9.8 * (A11+1293) * 1/1000</f>
         <v>22.471400000000003</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>2.847</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>3.3319999999999999</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>3.3620000000000001</v>
       </c>
       <c r="F11">
         <f>_xlfn.STDEV.P(C11:E11)</f>
         <v>0.23602024395283461</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f>AVERAGE(C11:E11)</f>
         <v>3.1803333333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="8">
+    <row r="12" spans="1:7">
+      <c r="A12" s="7">
         <v>800</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <f t="shared" ref="B12:B15" si="0">9.8 * (A12+1293) * 1/1000</f>
         <v>20.511400000000002</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>2.3919999999999999</v>
       </c>
       <c r="D12">
         <v>2.544</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>3.12</v>
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F15" si="1">_xlfn.STDEV.P(C12:E12)</f>
         <v>0.3135573667165571</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <f>AVERAGE(C12:E12)</f>
         <v>2.6853333333333338</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="8">
+    <row r="13" spans="1:7">
+      <c r="A13" s="7">
         <v>600</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>18.551400000000001</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>1.877</v>
       </c>
       <c r="D13">
         <v>1.726</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>1.786</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
         <v>6.2077013101111404E-2</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <f>AVERAGE(C13:E13)</f>
         <v>1.7963333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
+    <row r="14" spans="1:7">
+      <c r="A14" s="7">
         <v>400</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>16.5914</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>1.4830000000000001</v>
       </c>
       <c r="D14">
         <v>1.3320000000000001</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>1.3009999999999999</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
         <v>7.9502620501884558E-2</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <f>AVERAGE(C14:E14)</f>
         <v>1.3720000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="12">
+    <row r="15" spans="1:7">
+      <c r="A15" s="11">
         <v>200</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>14.631400000000001</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>0.93759999999999999</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>0.93759999999999999</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>0.9073</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
         <v>1.4283556979968257E-2</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <f>AVERAGE(C15:E15)</f>
         <v>0.92749999999999988</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C20" s="1" t="s">
+    <row r="20" spans="1:7">
+      <c r="C20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
         <v>1000</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <f>9.8 *(A22+1293) * 1/1000</f>
         <v>22.471400000000003</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>2.4049999999999998</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>2.35</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>2.407</v>
       </c>
       <c r="F22">
         <f>_xlfn.STDEV.P(C22:E22)</f>
         <v>2.6411277052720328E-2</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <f>AVERAGE(C22:E22)</f>
         <v>2.3873333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="8">
+    <row r="23" spans="1:7">
+      <c r="A23" s="7">
         <v>800</v>
       </c>
-      <c r="B23" s="3">
-        <f t="shared" ref="B23:B26" si="2">9.8 *(A23+1293) * 1/1000</f>
+      <c r="B23" s="2">
+        <f>9.8 *(A23+1293) * 1/1000</f>
         <v>20.511400000000002</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>2.0049999999999999</v>
       </c>
       <c r="D23">
         <v>1.887</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>1.97</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F26" si="3">_xlfn.STDEV.P(C23:E23)</f>
+        <f t="shared" ref="F23:F26" si="2">_xlfn.STDEV.P(C23:E23)</f>
         <v>4.9484004149489183E-2</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <f>AVERAGE(C23:E23)</f>
         <v>1.954</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="8">
+    <row r="24" spans="1:7">
+      <c r="A24" s="7">
         <v>600</v>
       </c>
-      <c r="B24" s="3">
-        <f t="shared" si="2"/>
+      <c r="B24" s="2">
+        <f t="shared" ref="B23:B26" si="3">9.8 *(A24+1293) * 1/1000</f>
         <v>18.551400000000001</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>1.5609999999999999</v>
       </c>
       <c r="D24">
         <v>1.5720000000000001</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>1.5609999999999999</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.1854497287014056E-3</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <f>AVERAGE(C24:E24)</f>
         <v>1.5646666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="8">
+    <row r="25" spans="1:7">
+      <c r="A25" s="7">
         <v>400</v>
       </c>
-      <c r="B25" s="3">
-        <f t="shared" si="2"/>
+      <c r="B25" s="2">
+        <f t="shared" si="3"/>
         <v>16.5914</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>1.115</v>
       </c>
       <c r="D25">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>1.131</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.3181661333666997E-3</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <f>AVERAGE(C25:E25)</f>
         <v>1.1253333333333335</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="12">
+    <row r="26" spans="1:7">
+      <c r="A26" s="11">
         <v>200</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
+        <f t="shared" si="3"/>
+        <v>14.631400000000001</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0.77480000000000004</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="F26">
         <f t="shared" si="2"/>
-        <v>14.631400000000001</v>
-      </c>
-      <c r="C26" s="13">
-        <v>0.77480000000000004</v>
-      </c>
-      <c r="D26" s="14">
-        <v>0.77490000000000003</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0.76870000000000005</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
         <v>2.8994252303976794E-3</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="15">
         <f>AVERAGE(C26:E26)</f>
         <v>0.77280000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="4">
+    <row r="34" spans="1:6">
+      <c r="A34" s="3">
         <v>1</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>1.9319999999999999</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="16">
         <f>B34 * $B$3</f>
         <v>2.4980759999999997</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <f>C34/ (9.8*$B$3)</f>
         <v>0.19714285714285712</v>
       </c>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="9">
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="8">
         <v>2</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <v>2.0609999999999999</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="18">
         <f>B35 * $B$3</f>
         <v>2.6648729999999996</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="10">
         <f>C35/ (9.8*$B$3)</f>
         <v>0.21030612244897956</v>
       </c>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="9">
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="8">
         <v>3</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>2.1030000000000002</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="18">
         <f>B36 * $B$3</f>
         <v>2.719179</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="10">
         <f>C36/ (9.8*$B$3)</f>
         <v>0.21459183673469387</v>
       </c>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="9">
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="8">
         <v>4</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>1.8160000000000001</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="18">
         <f>B37 * $B$3</f>
         <v>2.3480879999999997</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="10">
         <f>C37/ (9.8*$B$3)</f>
         <v>0.18530612244897957</v>
       </c>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="13">
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="12">
         <v>5</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <v>1.7230000000000001</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="19">
         <f>B38 * $B$3</f>
         <v>2.2278389999999999</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="15">
         <f>C38/ (9.8*$B$3)</f>
         <v>0.17581632653061224</v>
       </c>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C39" s="2" t="s">
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="20">
         <f>AVERAGE(D34:D38)</f>
         <v>0.19663265306122449</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="4">
+    <row r="45" spans="1:6">
+      <c r="A45" s="3">
         <v>1</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>2.0920000000000001</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="16">
         <f>B45 * $B$3</f>
         <v>2.7049560000000001</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <f>C45/ (9.8*$B$3+0.5)</f>
         <v>0.20536586847259974</v>
       </c>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="9">
+      <c r="F45" s="17"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="8">
         <v>2</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7">
         <v>1.8280000000000001</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="18">
         <f>B46 * $B$3</f>
         <v>2.363604</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="10">
         <f>C46/ (9.8*$B$3+0.5)</f>
         <v>0.17944971681066554</v>
       </c>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="9">
+      <c r="F46" s="17"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="8">
         <v>3</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>2.044</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="18">
         <f>B47 * $B$3</f>
         <v>2.6428919999999998</v>
       </c>
-      <c r="D47" s="11">
+      <c r="D47" s="10">
         <f>C47/ (9.8*$B$3+0.5)</f>
         <v>0.20065384089770258</v>
       </c>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="9">
+      <c r="F47" s="17"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="8">
         <v>4</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="18">
         <f>B48 * $B$3</f>
         <v>2.6247899999999995</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="10">
         <f>C48/ (9.8*$B$3+0.5)</f>
         <v>0.19927949952169088</v>
       </c>
-      <c r="F48" s="18"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="13">
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="12">
         <v>5</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="11">
         <v>2.0950000000000002</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="19">
         <f>B49 * $B$3</f>
         <v>2.7088350000000001</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D49" s="15">
         <f>C49/ (9.8*$B$3+0.5)</f>
         <v>0.20566037019603081</v>
       </c>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C50" s="2" t="s">
+      <c r="F49" s="17"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="C50" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="20">
         <f>AVERAGE(D45:D49)</f>
         <v>0.19808185917973792</v>
       </c>
@@ -3586,13 +3584,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BF56D4-6143-4B4E-A76C-39702C6372CB}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W51" sqref="W51"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3600,17 +3598,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:23">
+      <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A3" s="23">
+    <row r="3" spans="1:23">
+      <c r="A3" s="22">
         <v>1.2929999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3618,52 +3616,52 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="1:23" ht="14" thickBot="1">
+      <c r="C8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-    </row>
-    <row r="9" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:23" ht="14" thickBot="1">
+      <c r="A9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A10" s="24">
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
         <v>1000</v>
       </c>
       <c r="B10">
         <f>TRUNC((9.8*(A10+1293)*1/1000),4-(1+INT(LOG10(ABS((9.8*(A10+1293)*1/1000))))))</f>
         <v>22.47</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10">
         <v>2.847</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10">
         <v>3.3319999999999999</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10">
         <v>3.3620000000000001</v>
       </c>
       <c r="F10">
@@ -3674,23 +3672,22 @@
         <f>TRUNC(AVERAGE(C10:E10),4-(1+INT(LOG10(ABS((AVERAGE(C10:E10)))))))</f>
         <v>3.18</v>
       </c>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A11" s="24">
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
         <v>800</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B14" si="0">TRUNC((9.8*(A11+1293)*1/1000),4-(1+INT(LOG10(ABS((9.8*(A11+1293)*1/1000))))))</f>
         <v>20.51</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11">
         <v>2.3919999999999999</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11">
         <v>2.544</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11">
         <v>3.12</v>
       </c>
       <c r="F11">
@@ -3701,27 +3698,26 @@
         <f t="shared" ref="G11:G14" si="2">TRUNC(AVERAGE(C11:E11),4-(1+INT(LOG10(ABS((AVERAGE(C11:E11)))))))</f>
         <v>2.6850000000000001</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="K11" s="18">
+      <c r="K11" s="17">
         <f>TRUNC(C32,4-(1+INT(LOG10(ABS((C32))))))</f>
         <v>2.4980000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A12" s="24">
+    <row r="12" spans="1:23">
+      <c r="A12">
         <v>600</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>18.55</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12">
         <v>1.877</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12">
         <v>1.726</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12">
         <v>1.786</v>
       </c>
       <c r="F12">
@@ -3732,23 +3728,22 @@
         <f t="shared" si="2"/>
         <v>1.796</v>
       </c>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A13" s="24">
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13">
         <v>400</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>16.59</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13">
         <v>1.4830000000000001</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13">
         <v>1.3320000000000001</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13">
         <v>1.3009999999999999</v>
       </c>
       <c r="F13">
@@ -3759,26 +3754,25 @@
         <f t="shared" si="2"/>
         <v>1.3720000000000001</v>
       </c>
-      <c r="H13" s="24"/>
       <c r="W13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A14" s="24">
+    <row r="14" spans="1:23">
+      <c r="A14">
         <v>200</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
         <v>14.63</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14">
         <v>0.93759999999999999</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14">
         <v>0.93759999999999999</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14">
         <v>0.9073</v>
       </c>
       <c r="F14">
@@ -3789,66 +3783,61 @@
         <f t="shared" si="2"/>
         <v>0.92749999999999999</v>
       </c>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="24" t="s">
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="J18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="C19" s="27" t="s">
+    <row r="19" spans="1:10" ht="14" thickBot="1">
+      <c r="C19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="1:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:10" ht="14" thickBot="1">
+      <c r="A20" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="26"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="24">
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
         <v>1000</v>
       </c>
       <c r="B21">
         <f>TRUNC((9.8*(A21+1293)*1/1000),4-(1+INT(LOG10(ABS((9.8*(A21+1293)*1/1000))))))</f>
         <v>22.47</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21">
         <v>2.4049999999999998</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21">
         <v>2.35</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21">
         <v>2.407</v>
       </c>
       <c r="F21">
@@ -3859,23 +3848,22 @@
         <f>TRUNC(AVERAGE(C21:E21),4-(1+INT(LOG10(ABS((AVERAGE(C21:E21)))))))</f>
         <v>2.387</v>
       </c>
-      <c r="H21" s="24"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="24">
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
         <v>800</v>
       </c>
       <c r="B22">
         <f t="shared" ref="B22:B25" si="3">TRUNC((9.8*(A22+1293)*1/1000),4-(1+INT(LOG10(ABS((9.8*(A22+1293)*1/1000))))))</f>
         <v>20.51</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22">
         <v>2.0049999999999999</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22">
         <v>1.887</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22">
         <v>1.97</v>
       </c>
       <c r="F22">
@@ -3886,23 +3874,22 @@
         <f t="shared" ref="G22:G25" si="5">TRUNC(AVERAGE(C22:E22),4-(1+INT(LOG10(ABS((AVERAGE(C22:E22)))))))</f>
         <v>1.954</v>
       </c>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="24">
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
         <v>600</v>
       </c>
       <c r="B23">
         <f t="shared" si="3"/>
         <v>18.55</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23">
         <v>1.5609999999999999</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23">
         <v>1.5720000000000001</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23">
         <v>1.5609999999999999</v>
       </c>
       <c r="F23">
@@ -3913,23 +3900,22 @@
         <f t="shared" si="5"/>
         <v>1.5640000000000001</v>
       </c>
-      <c r="H23" s="24"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="24">
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
         <v>400</v>
       </c>
       <c r="B24">
         <f t="shared" si="3"/>
         <v>16.59</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24">
         <v>1.115</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24">
         <v>1.131</v>
       </c>
       <c r="F24">
@@ -3940,23 +3926,22 @@
         <f t="shared" si="5"/>
         <v>1.125</v>
       </c>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" s="24">
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
         <v>200</v>
       </c>
       <c r="B25">
         <f t="shared" si="3"/>
         <v>14.63</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25">
         <v>0.77480000000000004</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25">
         <v>0.77490000000000003</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25">
         <v>0.76870000000000005</v>
       </c>
       <c r="F25">
@@ -3967,9 +3952,8 @@
         <f t="shared" si="5"/>
         <v>0.77280000000000004</v>
       </c>
-      <c r="H25" s="24"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -3977,251 +3961,251 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:10">
+      <c r="A31" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" s="24">
+    <row r="32" spans="1:10">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" s="24">
+      <c r="B32">
         <v>1.9319999999999999</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="17">
         <v>2.4980000000000002</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="17">
         <v>0.19714285714285712</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="17">
         <f>TRUNC(C32,4-(1+INT(LOG10(ABS(C32)))))</f>
         <v>2.4980000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="24">
+    <row r="33" spans="1:6">
+      <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33">
         <v>2.0609999999999999</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="17">
         <v>2.6640000000000001</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="17">
         <v>0.21030612244897956</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="17">
         <f t="shared" ref="F33:F36" si="6">TRUNC(C33,4-(1+INT(LOG10(ABS(C33)))))</f>
         <v>2.6640000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="24">
+    <row r="34" spans="1:6">
+      <c r="A34">
         <v>3</v>
       </c>
-      <c r="B34" s="24">
+      <c r="B34">
         <v>2.1030000000000002</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="17">
         <v>2.7189999999999999</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="17">
         <v>0.21459183673469387</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="17">
         <f t="shared" si="6"/>
         <v>2.7189999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="24">
+    <row r="35" spans="1:6">
+      <c r="A35">
         <v>4</v>
       </c>
-      <c r="B35" s="24">
+      <c r="B35">
         <v>1.8160000000000001</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="17">
         <v>2.3479999999999999</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="17">
         <v>0.18530612244897957</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="17">
         <f t="shared" si="6"/>
         <v>2.3479999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="14">
+    <row r="36" spans="1:6">
+      <c r="A36" s="13">
         <v>5</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="13">
         <v>1.7230000000000001</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36" s="24">
         <v>2.2269999999999999</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="24">
         <v>0.17581632653061224</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="17">
         <f t="shared" si="6"/>
         <v>2.2269999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C37" s="30" t="s">
+    <row r="37" spans="1:6">
+      <c r="C37" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="25">
         <v>0.19663265306122449</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6">
       <c r="B39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="30" t="s">
+    <row r="41" spans="1:6">
+      <c r="A41" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="24">
+    <row r="42" spans="1:6">
+      <c r="A42">
         <v>1</v>
       </c>
-      <c r="B42" s="24">
+      <c r="B42">
         <v>2.0920000000000001</v>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="17">
         <v>2.7040000000000002</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="17">
         <v>0.20536586847259974</v>
       </c>
-      <c r="F42" s="18">
+      <c r="F42" s="17">
         <f>TRUNC(C42,4-(1+INT(LOG10(ABS(C42)))))</f>
         <v>2.7040000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="24">
+    <row r="43" spans="1:6">
+      <c r="A43">
         <v>2</v>
       </c>
-      <c r="B43" s="24">
+      <c r="B43">
         <v>1.8280000000000001</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="17">
         <v>2.363</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="17">
         <v>0.17944971681066554</v>
       </c>
-      <c r="F43" s="18">
+      <c r="F43" s="17">
         <f t="shared" ref="F43:F46" si="7">TRUNC(C43,4-(1+INT(LOG10(ABS(C43)))))</f>
         <v>2.363</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="24">
+    <row r="44" spans="1:6">
+      <c r="A44">
         <v>3</v>
       </c>
-      <c r="B44" s="24">
+      <c r="B44">
         <v>2.044</v>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="17">
         <v>2.6419999999999999</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="17">
         <v>0.20065384089770258</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="17">
         <f t="shared" si="7"/>
         <v>2.6419999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="24">
+    <row r="45" spans="1:6">
+      <c r="A45">
         <v>4</v>
       </c>
-      <c r="B45" s="24">
+      <c r="B45">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="17">
         <v>2.6240000000000001</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="17">
         <v>0.19927949952169088</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="17">
         <f t="shared" si="7"/>
         <v>2.6240000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="14">
+    <row r="46" spans="1:6">
+      <c r="A46" s="13">
         <v>5</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="13">
         <v>2.0950000000000002</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C46" s="24">
         <v>2.7080000000000002</v>
       </c>
-      <c r="D46" s="28">
+      <c r="D46" s="24">
         <v>0.20566037019603081</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="17">
         <f t="shared" si="7"/>
         <v>2.7080000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C47" s="30" t="s">
+    <row r="47" spans="1:6">
+      <c r="C47" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="25">
         <v>0.19808185917973792</v>
       </c>
     </row>
-    <row r="50" spans="8:23" x14ac:dyDescent="0.15">
+    <row r="50" spans="8:23">
       <c r="W50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="8:23" x14ac:dyDescent="0.15">
+    <row r="61" spans="8:23">
       <c r="H61" t="s">
         <v>38</v>
       </c>

</xml_diff>